<commit_message>
saved plane name to mic_coords_final
</commit_message>
<xml_diff>
--- a/mic_positions/data/mic_coords_final.xlsx
+++ b/mic_positions/data/mic_coords_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,45 +441,50 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Plane</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>X</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Z</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>X_optimized</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Y_optimized</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Z_optimized</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Array_Channel</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Stagebox</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Stagebox_Channel</t>
         </is>
@@ -494,33 +499,38 @@
           <t>B1</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>1.37</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>0.8139999999999998</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.02</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>1.431736970439887</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.7724205632644902</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.03016703382869369</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>1</v>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -533,33 +543,38 @@
           <t>B2</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>1.37</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.5609999999999998</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.266</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>1.422030911618047</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.5195226985835854</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.2760805602195486</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>2</v>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -572,33 +587,38 @@
           <t>B3</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>1.37</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>1.212</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.287</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>1.429668287755774</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>1.170478135207909</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.2970731783260849</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>3</v>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>3</v>
       </c>
     </row>
@@ -611,33 +631,38 @@
           <t>B4</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>1.37</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>0.15</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.38</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>1.413835492859852</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>0.1085933005350677</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>0.3900404870836032</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>4</v>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>4</v>
       </c>
     </row>
@@ -650,33 +675,38 @@
           <t>B5</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>1.37</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>0.9009999999999998</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>0.425</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>1.422095312390745</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>0.8595488243725178</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>0.4350246687404669</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>5</v>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>5</v>
       </c>
     </row>
@@ -689,33 +719,38 @@
           <t>B6</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>1.37</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>0.5589999999999998</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.629</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>1.412382454086071</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>0.5176439942681164</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>0.638952958918249</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>6</v>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>6</v>
       </c>
     </row>
@@ -728,33 +763,38 @@
           <t>B7</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>1.37</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>1.326</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>0.672</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>1.420896685431991</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>1.284597583184944</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>0.6819378436125855</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>7</v>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>7</v>
       </c>
     </row>
@@ -767,33 +807,38 @@
           <t>B8</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>1.37</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>0.2329999999999999</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>0.718</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>1.405919685430265</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>0.1916995198520569</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>0.7279216737507128</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>8</v>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>8</v>
       </c>
     </row>
@@ -806,33 +851,38 @@
           <t>B9</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>1.37</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>0.9209999999999998</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>0.774</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>1.41309491336665</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>0.8796637052876608</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>0.7839019887014765</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>9</v>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>9</v>
       </c>
     </row>
@@ -845,33 +895,38 @@
           <t>B10</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
         <v>1.37</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>1.174</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>0.989</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>1.41057966704335</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>1.132715410935535</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>0.9988264121731586</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>10</v>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>10</v>
       </c>
     </row>
@@ -884,33 +939,38 @@
           <t>B11</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>1.37</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>0.3779999999999999</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>1.148</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>1.396345309058903</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>0.336831529066288</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>1.157770520694077</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>11</v>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>11</v>
       </c>
     </row>
@@ -923,33 +983,38 @@
           <t>B12</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>1.37</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>0.7389999999999999</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>1.194</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>1.399669713311482</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>0.6978182818733589</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>1.203754350832204</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>12</v>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>12</v>
       </c>
     </row>
@@ -962,33 +1027,38 @@
           <t>B13</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>1.37</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>1.391</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>1.257</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>1.406206238605785</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>1.349787655158926</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>1.266732205151814</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>13</v>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1001,33 +1071,38 @@
           <t>B14</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
         <v>1.37</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>1.012</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>1.372</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>1.398387091361103</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>0.9708560558262891</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>1.381691780497132</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>14</v>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1040,33 +1115,38 @@
           <t>B15</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
         <v>1.37</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>0.5039999999999999</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>1.485</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>1.388997250280228</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>0.4629340082715897</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>1.494652058879923</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>15</v>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>15</v>
       </c>
     </row>
@@ -1079,33 +1159,38 @@
           <t>B16</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
         <v>1.37</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>0.156</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>1.51</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>1.383954236134591</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>0.1149699191337609</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>1.519643270911514</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>16</v>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>right</t>
         </is>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1118,33 +1203,38 @@
           <t>C1</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
         <v>0.7389999999999999</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>0.028</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>0.023</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>0.7469338968689182</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>0.01005461907086658</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>0.03299039662966993</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>17</v>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1157,33 +1247,38 @@
           <t>C2</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
         <v>0.4849999999999999</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>0.028</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>0.267</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>0.4928336155895092</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>0.008528993191660318</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>0.2768811908786574</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>18</v>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="K19" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1196,33 +1291,38 @@
           <t>C3</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
         <v>1.137</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>0.028</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>0.287</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>1.144651661547618</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>-0.006885056726207126</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>0.2968722395875908</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>19</v>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="K20" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1235,33 +1335,38 @@
           <t>C4</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
         <v>0.07599999999999983</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>0.028</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>0.38</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>0.08386241058151087</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>0.01444345175174852</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>0.3898306160841312</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>20</v>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="K21" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1274,33 +1379,38 @@
           <t>C5</t>
         </is>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
         <v>0.8269999999999998</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>0.028</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>0.425</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>0.8346378981974144</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>-0.003967942163637914</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>0.4348104756792313</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>21</v>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="K22" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K22" t="n">
+      <c r="L22" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1313,33 +1423,38 @@
           <t>C6</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
         <v>0.4839999999999999</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>0.028</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>0.63</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>0.49158711013476</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>-0.002304754831412761</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>0.6397187249457987</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>22</v>
       </c>
-      <c r="J23" t="inlineStr">
+      <c r="K23" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K23" t="n">
+      <c r="L23" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1352,33 +1467,38 @@
           <t>C7</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
         <v>1.252</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>0.028</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>0.675</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>1.259358208041763</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>-0.02110245281495124</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>0.6846985845408989</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>23</v>
       </c>
-      <c r="J24" t="inlineStr">
+      <c r="K24" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K24" t="n">
+      <c r="L24" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1391,33 +1511,38 @@
           <t>C8</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
         <v>0.1569999999999998</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>0.028</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>0.717</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>0.1646124057698179</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>0.002523953224601003</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>0.7266797868296591</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>24</v>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="K25" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K25" t="n">
+      <c r="L25" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1430,33 +1555,38 @@
           <t>C9</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
         <v>0.8459999999999999</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>0.028</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>0.773</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>0.8533964252252414</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>-0.01480755102415678</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>0.7826547232146726</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>25</v>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="K26" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K26" t="n">
+      <c r="L26" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1469,33 +1599,38 @@
           <t>C10</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
         <v>1.099</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>0.028</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>0.99</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>1.10618358165611</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>-0.02704662147544842</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>0.9995576017066</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>26</v>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="K27" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K27" t="n">
+      <c r="L27" t="n">
         <v>10</v>
       </c>
     </row>
@@ -1508,33 +1643,38 @@
           <t>C11</t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
         <v>0.3039999999999998</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>0.028</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>1.15</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>0.3112800987445385</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>-0.01376644707356975</v>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>1.159485991378067</v>
       </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
         <v>27</v>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="K28" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K28" t="n">
+      <c r="L28" t="n">
         <v>11</v>
       </c>
     </row>
@@ -1547,33 +1687,38 @@
           <t>C12</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
         <v>0.6669999999999999</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>0.028</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>1.194</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>0.674156454800373</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>-0.02333111109181371</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>1.203466298537721</v>
       </c>
-      <c r="I29" t="n">
+      <c r="J29" t="n">
         <v>28</v>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="K29" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K29" t="n">
+      <c r="L29" t="n">
         <v>12</v>
       </c>
     </row>
@@ -1586,33 +1731,38 @@
           <t>C13</t>
         </is>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
         <v>1.313</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>0.028</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>1.261</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>1.319944099950075</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>-0.04001447727952451</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>1.270436311712648</v>
       </c>
-      <c r="I30" t="n">
+      <c r="J30" t="n">
         <v>29</v>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="K30" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K30" t="n">
+      <c r="L30" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1625,33 +1775,38 @@
           <t>C14</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
         <v>0.9369999999999998</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>0.028</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>1.375</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>0.9439636939527135</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>-0.03487981072281562</v>
       </c>
-      <c r="H31" t="n">
+      <c r="I31" t="n">
         <v>1.384385289353568</v>
       </c>
-      <c r="I31" t="n">
+      <c r="J31" t="n">
         <v>30</v>
       </c>
-      <c r="J31" t="inlineStr">
+      <c r="K31" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K31" t="n">
+      <c r="L31" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1664,33 +1819,38 @@
           <t>C15</t>
         </is>
       </c>
-      <c r="C32" t="n">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
         <v>0.4189999999999999</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>0.028</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>1.485</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>0.4260226740945098</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>-0.02639873846544125</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>1.494336057252702</v>
       </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
         <v>31</v>
       </c>
-      <c r="J32" t="inlineStr">
+      <c r="K32" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K32" t="n">
+      <c r="L32" t="n">
         <v>15</v>
       </c>
     </row>
@@ -1703,33 +1863,38 @@
           <t>C16</t>
         </is>
       </c>
-      <c r="C33" t="n">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
         <v>0.08499999999999995</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
         <v>0.028</v>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>1.508</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>0.09209328379964611</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>-0.01949687533786055</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>1.517325763267975</v>
       </c>
-      <c r="I33" t="n">
+      <c r="J33" t="n">
         <v>32</v>
       </c>
-      <c r="J33" t="inlineStr">
+      <c r="K33" t="inlineStr">
         <is>
           <t>front</t>
         </is>
       </c>
-      <c r="K33" t="n">
+      <c r="L33" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1742,33 +1907,38 @@
           <t>D1</t>
         </is>
       </c>
-      <c r="C34" t="n">
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
         <v>0.028</v>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="n">
         <v>0.737</v>
       </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
         <v>0.023</v>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>0.0382713656488418</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>0.6994046470141787</v>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>0.01063476537521875</v>
       </c>
-      <c r="I34" t="n">
+      <c r="J34" t="n">
         <v>33</v>
       </c>
-      <c r="J34" t="inlineStr">
+      <c r="K34" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K34" t="n">
+      <c r="L34" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1781,33 +1951,38 @@
           <t>D2</t>
         </is>
       </c>
-      <c r="C35" t="n">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
         <v>0.028</v>
       </c>
-      <c r="D35" t="n">
+      <c r="E35" t="n">
         <v>0.988</v>
       </c>
-      <c r="E35" t="n">
+      <c r="F35" t="n">
         <v>0.27</v>
       </c>
-      <c r="F35" t="n">
+      <c r="G35" t="n">
         <v>0.03830999191730931</v>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>0.9504319503401228</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>0.2576070138018707</v>
       </c>
-      <c r="I35" t="n">
+      <c r="J35" t="n">
         <v>34</v>
       </c>
-      <c r="J35" t="inlineStr">
+      <c r="K35" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K35" t="n">
+      <c r="L35" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1820,33 +1995,38 @@
           <t>D3</t>
         </is>
       </c>
-      <c r="C36" t="n">
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
         <v>0.028</v>
       </c>
-      <c r="D36" t="n">
+      <c r="E36" t="n">
         <v>0.339</v>
       </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
         <v>0.289</v>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>0.02835300806285724</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>0.3015082725567115</v>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>0.2766048790654592</v>
       </c>
-      <c r="I36" t="n">
+      <c r="J36" t="n">
         <v>35</v>
       </c>
-      <c r="J36" t="inlineStr">
+      <c r="K36" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K36" t="n">
+      <c r="L36" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1859,33 +2039,38 @@
           <t>D4</t>
         </is>
       </c>
-      <c r="C37" t="n">
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
         <v>0.028</v>
       </c>
-      <c r="D37" t="n">
+      <c r="E37" t="n">
         <v>1.4</v>
       </c>
-      <c r="E37" t="n">
+      <c r="F37" t="n">
         <v>0.385</v>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>0.04272648535037085</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>1.362411884556102</v>
       </c>
-      <c r="H37" t="n">
+      <c r="I37" t="n">
         <v>0.3725940930288543</v>
       </c>
-      <c r="I37" t="n">
+      <c r="J37" t="n">
         <v>36</v>
       </c>
-      <c r="J37" t="inlineStr">
+      <c r="K37" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K37" t="n">
+      <c r="L37" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1898,33 +2083,38 @@
           <t>D5</t>
         </is>
       </c>
-      <c r="C38" t="n">
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
         <v>0.028</v>
       </c>
-      <c r="D38" t="n">
+      <c r="E38" t="n">
         <v>0.649</v>
       </c>
-      <c r="E38" t="n">
+      <c r="F38" t="n">
         <v>0.427</v>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>0.03090464129903687</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>0.6115046729994396</v>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>0.4145893741378396</v>
       </c>
-      <c r="I38" t="n">
+      <c r="J38" t="n">
         <v>37</v>
       </c>
-      <c r="J38" t="inlineStr">
+      <c r="K38" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K38" t="n">
+      <c r="L38" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1937,33 +2127,38 @@
           <t>D6</t>
         </is>
       </c>
-      <c r="C39" t="n">
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
         <v>0.028</v>
       </c>
-      <c r="D39" t="n">
+      <c r="E39" t="n">
         <v>0.992</v>
       </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
         <v>0.63</v>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>0.03297384778578524</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>0.9545119293387857</v>
       </c>
-      <c r="H39" t="n">
+      <c r="I39" t="n">
         <v>0.6175665661646021</v>
       </c>
-      <c r="I39" t="n">
+      <c r="J39" t="n">
         <v>38</v>
       </c>
-      <c r="J39" t="inlineStr">
+      <c r="K39" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K39" t="n">
+      <c r="L39" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1976,33 +2171,38 @@
           <t>D7</t>
         </is>
       </c>
-      <c r="C40" t="n">
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
         <v>0.028</v>
       </c>
-      <c r="D40" t="n">
+      <c r="E40" t="n">
         <v>0.223</v>
       </c>
-      <c r="E40" t="n">
+      <c r="F40" t="n">
         <v>0.677</v>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>0.02080880420396231</v>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>0.1856078338436715</v>
       </c>
-      <c r="H40" t="n">
+      <c r="I40" t="n">
         <v>0.6645612855008477</v>
       </c>
-      <c r="I40" t="n">
+      <c r="J40" t="n">
         <v>39</v>
       </c>
-      <c r="J40" t="inlineStr">
+      <c r="K40" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K40" t="n">
+      <c r="L40" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2015,33 +2215,38 @@
           <t>D8</t>
         </is>
       </c>
-      <c r="C41" t="n">
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
         <v>0.028</v>
       </c>
-      <c r="D41" t="n">
+      <c r="E41" t="n">
         <v>1.317</v>
       </c>
-      <c r="E41" t="n">
+      <c r="F41" t="n">
         <v>0.72</v>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>0.03646846402108281</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>1.279495940789802</v>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>0.707556454255285</v>
       </c>
-      <c r="I41" t="n">
+      <c r="J41" t="n">
         <v>40</v>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="K41" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K41" t="n">
+      <c r="L41" t="n">
         <v>8</v>
       </c>
     </row>
@@ -2054,33 +2259,38 @@
           <t>D9</t>
         </is>
       </c>
-      <c r="C42" t="n">
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
         <v>0.028</v>
       </c>
-      <c r="D42" t="n">
+      <c r="E42" t="n">
         <v>0.629</v>
       </c>
-      <c r="E42" t="n">
+      <c r="F42" t="n">
         <v>0.773</v>
       </c>
-      <c r="F42" t="n">
+      <c r="G42" t="n">
         <v>0.02542065422092971</v>
       </c>
-      <c r="G42" t="n">
+      <c r="H42" t="n">
         <v>0.5915841898573074</v>
       </c>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
         <v>0.7605504994642427</v>
       </c>
-      <c r="I42" t="n">
+      <c r="J42" t="n">
         <v>41</v>
       </c>
-      <c r="J42" t="inlineStr">
+      <c r="K42" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K42" t="n">
+      <c r="L42" t="n">
         <v>9</v>
       </c>
     </row>
@@ -2093,33 +2303,38 @@
           <t>D10</t>
         </is>
       </c>
-      <c r="C43" t="n">
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
         <v>0.028</v>
       </c>
-      <c r="D43" t="n">
+      <c r="E43" t="n">
         <v>0.377</v>
       </c>
-      <c r="E43" t="n">
+      <c r="F43" t="n">
         <v>0.99</v>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>0.01841259330240147</v>
       </c>
-      <c r="G43" t="n">
+      <c r="H43" t="n">
         <v>0.3396606542073992</v>
       </c>
-      <c r="H43" t="n">
+      <c r="I43" t="n">
         <v>0.9775261185273336</v>
       </c>
-      <c r="I43" t="n">
+      <c r="J43" t="n">
         <v>42</v>
       </c>
-      <c r="J43" t="inlineStr">
+      <c r="K43" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K43" t="n">
+      <c r="L43" t="n">
         <v>10</v>
       </c>
     </row>
@@ -2132,33 +2347,38 @@
           <t>D11</t>
         </is>
       </c>
-      <c r="C44" t="n">
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
         <v>0.028</v>
       </c>
-      <c r="D44" t="n">
+      <c r="E44" t="n">
         <v>1.17</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>1.149</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>0.02784774269881322</v>
       </c>
-      <c r="G44" t="n">
+      <c r="H44" t="n">
         <v>1.132608104236331</v>
       </c>
-      <c r="H44" t="n">
+      <c r="I44" t="n">
         <v>1.136508254154207</v>
       </c>
-      <c r="I44" t="n">
+      <c r="J44" t="n">
         <v>43</v>
       </c>
-      <c r="J44" t="inlineStr">
+      <c r="K44" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K44" t="n">
+      <c r="L44" t="n">
         <v>11</v>
       </c>
     </row>
@@ -2171,33 +2391,38 @@
           <t>D12</t>
         </is>
       </c>
-      <c r="C45" t="n">
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
         <v>0.028</v>
       </c>
-      <c r="D45" t="n">
+      <c r="E45" t="n">
         <v>0.8079999999999999</v>
       </c>
-      <c r="E45" t="n">
+      <c r="F45" t="n">
         <v>1.195</v>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>0.02176330916192526</v>
       </c>
-      <c r="G45" t="n">
+      <c r="H45" t="n">
         <v>0.7706585841008975</v>
       </c>
-      <c r="H45" t="n">
+      <c r="I45" t="n">
         <v>1.182503085845</v>
       </c>
-      <c r="I45" t="n">
+      <c r="J45" t="n">
         <v>44</v>
       </c>
-      <c r="J45" t="inlineStr">
+      <c r="K45" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K45" t="n">
+      <c r="L45" t="n">
         <v>12</v>
       </c>
     </row>
@@ -2210,33 +2435,38 @@
           <t>D13</t>
         </is>
       </c>
-      <c r="C46" t="n">
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
         <v>0.028</v>
       </c>
-      <c r="D46" t="n">
+      <c r="E46" t="n">
         <v>0.162</v>
       </c>
-      <c r="E46" t="n">
+      <c r="F46" t="n">
         <v>1.26</v>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>0.01116157719615678</v>
       </c>
-      <c r="G46" t="n">
+      <c r="H46" t="n">
         <v>0.1247448494412902</v>
       </c>
-      <c r="H46" t="n">
+      <c r="I46" t="n">
         <v>1.247495782799382</v>
       </c>
-      <c r="I46" t="n">
+      <c r="J46" t="n">
         <v>45</v>
       </c>
-      <c r="J46" t="inlineStr">
+      <c r="K46" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K46" t="n">
+      <c r="L46" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2249,33 +2479,38 @@
           <t>D14</t>
         </is>
       </c>
-      <c r="C47" t="n">
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
         <v>0.028</v>
       </c>
-      <c r="D47" t="n">
+      <c r="E47" t="n">
         <v>0.538</v>
       </c>
-      <c r="E47" t="n">
+      <c r="F47" t="n">
         <v>1.375</v>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>0.01504155371053182</v>
       </c>
-      <c r="G47" t="n">
+      <c r="H47" t="n">
         <v>0.5007287818015643</v>
       </c>
-      <c r="H47" t="n">
+      <c r="I47" t="n">
         <v>1.362482862026366</v>
       </c>
-      <c r="I47" t="n">
+      <c r="J47" t="n">
         <v>46</v>
       </c>
-      <c r="J47" t="inlineStr">
+      <c r="K47" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K47" t="n">
+      <c r="L47" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2288,33 +2523,38 @@
           <t>D15</t>
         </is>
       </c>
-      <c r="C48" t="n">
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
         <v>0.028</v>
       </c>
-      <c r="D48" t="n">
+      <c r="E48" t="n">
         <v>1.051</v>
       </c>
-      <c r="E48" t="n">
+      <c r="F48" t="n">
         <v>1.485</v>
       </c>
-      <c r="F48" t="n">
+      <c r="G48" t="n">
         <v>0.02103821623660954</v>
       </c>
-      <c r="G48" t="n">
+      <c r="H48" t="n">
         <v>1.013696382012205</v>
       </c>
-      <c r="H48" t="n">
+      <c r="I48" t="n">
         <v>1.47247050302609</v>
       </c>
-      <c r="I48" t="n">
+      <c r="J48" t="n">
         <v>47</v>
       </c>
-      <c r="J48" t="inlineStr">
+      <c r="K48" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K48" t="n">
+      <c r="L48" t="n">
         <v>15</v>
       </c>
     </row>
@@ -2327,33 +2567,38 @@
           <t>D16</t>
         </is>
       </c>
-      <c r="C49" t="n">
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
         <v>0.028</v>
       </c>
-      <c r="D49" t="n">
+      <c r="E49" t="n">
         <v>1.393</v>
       </c>
-      <c r="E49" t="n">
+      <c r="F49" t="n">
         <v>1.511</v>
       </c>
-      <c r="F49" t="n">
+      <c r="G49" t="n">
         <v>0.02574543339417382</v>
       </c>
-      <c r="G49" t="n">
+      <c r="H49" t="n">
         <v>1.355664207986297</v>
       </c>
-      <c r="H49" t="n">
+      <c r="I49" t="n">
         <v>1.498467581807842</v>
       </c>
-      <c r="I49" t="n">
+      <c r="J49" t="n">
         <v>48</v>
       </c>
-      <c r="J49" t="inlineStr">
+      <c r="K49" t="inlineStr">
         <is>
           <t>left</t>
         </is>
       </c>
-      <c r="K49" t="n">
+      <c r="L49" t="n">
         <v>16</v>
       </c>
     </row>
@@ -2366,33 +2611,38 @@
           <t>A1</t>
         </is>
       </c>
-      <c r="C50" t="n">
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
         <v>0.89</v>
       </c>
-      <c r="D50" t="n">
+      <c r="E50" t="n">
         <v>1.246</v>
       </c>
-      <c r="E50" t="n">
+      <c r="F50" t="n">
         <v>1.871</v>
       </c>
-      <c r="F50" t="n">
+      <c r="G50" t="n">
         <v>0.8493005129940666</v>
       </c>
-      <c r="G50" t="n">
+      <c r="H50" t="n">
         <v>1.21166964630419</v>
       </c>
-      <c r="H50" t="n">
+      <c r="I50" t="n">
         <v>1.871</v>
       </c>
-      <c r="I50" t="n">
+      <c r="J50" t="n">
         <v>49</v>
       </c>
-      <c r="J50" t="inlineStr">
+      <c r="K50" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K50" t="n">
+      <c r="L50" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2405,33 +2655,38 @@
           <t>A2</t>
         </is>
       </c>
-      <c r="C51" t="n">
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
         <v>0.321</v>
       </c>
-      <c r="D51" t="n">
+      <c r="E51" t="n">
         <v>1.147</v>
       </c>
-      <c r="E51" t="n">
+      <c r="F51" t="n">
         <v>1.871</v>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>0.2803005129940666</v>
       </c>
-      <c r="G51" t="n">
+      <c r="H51" t="n">
         <v>1.11266964630419</v>
       </c>
-      <c r="H51" t="n">
+      <c r="I51" t="n">
         <v>1.871</v>
       </c>
-      <c r="I51" t="n">
+      <c r="J51" t="n">
         <v>50</v>
       </c>
-      <c r="J51" t="inlineStr">
+      <c r="K51" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K51" t="n">
+      <c r="L51" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2444,33 +2699,38 @@
           <t>A3</t>
         </is>
       </c>
-      <c r="C52" t="n">
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
         <v>0.61</v>
       </c>
-      <c r="D52" t="n">
+      <c r="E52" t="n">
         <v>1.127</v>
       </c>
-      <c r="E52" t="n">
+      <c r="F52" t="n">
         <v>1.871</v>
       </c>
-      <c r="F52" t="n">
+      <c r="G52" t="n">
         <v>0.5693005129940666</v>
       </c>
-      <c r="G52" t="n">
+      <c r="H52" t="n">
         <v>1.09266964630419</v>
       </c>
-      <c r="H52" t="n">
+      <c r="I52" t="n">
         <v>1.871</v>
       </c>
-      <c r="I52" t="n">
+      <c r="J52" t="n">
         <v>51</v>
       </c>
-      <c r="J52" t="inlineStr">
+      <c r="K52" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K52" t="n">
+      <c r="L52" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2483,33 +2743,38 @@
           <t>A4</t>
         </is>
       </c>
-      <c r="C53" t="n">
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
         <v>0.104</v>
       </c>
-      <c r="D53" t="n">
+      <c r="E53" t="n">
         <v>0.8640000000000001</v>
       </c>
-      <c r="E53" t="n">
+      <c r="F53" t="n">
         <v>1.871</v>
       </c>
-      <c r="F53" t="n">
+      <c r="G53" t="n">
         <v>0.06330051299406655</v>
       </c>
-      <c r="G53" t="n">
+      <c r="H53" t="n">
         <v>0.8296696463041897</v>
       </c>
-      <c r="H53" t="n">
+      <c r="I53" t="n">
         <v>1.871</v>
       </c>
-      <c r="I53" t="n">
+      <c r="J53" t="n">
         <v>52</v>
       </c>
-      <c r="J53" t="inlineStr">
+      <c r="K53" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K53" t="n">
+      <c r="L53" t="n">
         <v>4</v>
       </c>
     </row>
@@ -2522,33 +2787,38 @@
           <t>A5</t>
         </is>
       </c>
-      <c r="C54" t="n">
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
         <v>0.452</v>
       </c>
-      <c r="D54" t="n">
+      <c r="E54" t="n">
         <v>0.857</v>
       </c>
-      <c r="E54" t="n">
+      <c r="F54" t="n">
         <v>1.871</v>
       </c>
-      <c r="F54" t="n">
+      <c r="G54" t="n">
         <v>0.4113005129940666</v>
       </c>
-      <c r="G54" t="n">
+      <c r="H54" t="n">
         <v>0.8226696463041896</v>
       </c>
-      <c r="H54" t="n">
+      <c r="I54" t="n">
         <v>1.871</v>
       </c>
-      <c r="I54" t="n">
+      <c r="J54" t="n">
         <v>53</v>
       </c>
-      <c r="J54" t="inlineStr">
+      <c r="K54" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K54" t="n">
+      <c r="L54" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2561,33 +2831,38 @@
           <t>A6</t>
         </is>
       </c>
-      <c r="C55" t="n">
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
         <v>1.069</v>
       </c>
-      <c r="D55" t="n">
+      <c r="E55" t="n">
         <v>0.8560000000000001</v>
       </c>
-      <c r="E55" t="n">
+      <c r="F55" t="n">
         <v>1.871</v>
       </c>
-      <c r="F55" t="n">
+      <c r="G55" t="n">
         <v>1.028300512994067</v>
       </c>
-      <c r="G55" t="n">
+      <c r="H55" t="n">
         <v>0.8216696463041897</v>
       </c>
-      <c r="H55" t="n">
+      <c r="I55" t="n">
         <v>1.871</v>
       </c>
-      <c r="I55" t="n">
+      <c r="J55" t="n">
         <v>54</v>
       </c>
-      <c r="J55" t="inlineStr">
+      <c r="K55" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K55" t="n">
+      <c r="L55" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2600,33 +2875,38 @@
           <t>A7</t>
         </is>
       </c>
-      <c r="C56" t="n">
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
         <v>0.725</v>
       </c>
-      <c r="D56" t="n">
+      <c r="E56" t="n">
         <v>0.8100000000000001</v>
       </c>
-      <c r="E56" t="n">
+      <c r="F56" t="n">
         <v>1.871</v>
       </c>
-      <c r="F56" t="n">
+      <c r="G56" t="n">
         <v>0.6843005129940666</v>
       </c>
-      <c r="G56" t="n">
+      <c r="H56" t="n">
         <v>0.7756696463041897</v>
       </c>
-      <c r="H56" t="n">
+      <c r="I56" t="n">
         <v>1.871</v>
       </c>
-      <c r="I56" t="n">
+      <c r="J56" t="n">
         <v>55</v>
       </c>
-      <c r="J56" t="inlineStr">
+      <c r="K56" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K56" t="n">
+      <c r="L56" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2639,33 +2919,38 @@
           <t>A8</t>
         </is>
       </c>
-      <c r="C57" t="n">
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
         <v>0.506</v>
       </c>
-      <c r="D57" t="n">
+      <c r="E57" t="n">
         <v>0.548</v>
       </c>
-      <c r="E57" t="n">
+      <c r="F57" t="n">
         <v>1.871</v>
       </c>
-      <c r="F57" t="n">
+      <c r="G57" t="n">
         <v>0.4653005129940666</v>
       </c>
-      <c r="G57" t="n">
+      <c r="H57" t="n">
         <v>0.5136696463041897</v>
       </c>
-      <c r="H57" t="n">
+      <c r="I57" t="n">
         <v>1.871</v>
       </c>
-      <c r="I57" t="n">
+      <c r="J57" t="n">
         <v>56</v>
       </c>
-      <c r="J57" t="inlineStr">
+      <c r="K57" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K57" t="n">
+      <c r="L57" t="n">
         <v>8</v>
       </c>
     </row>
@@ -2678,33 +2963,38 @@
           <t>A9</t>
         </is>
       </c>
-      <c r="C58" t="n">
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
         <v>0.07499999999999994</v>
       </c>
-      <c r="D58" t="n">
+      <c r="E58" t="n">
         <v>0.5209999999999999</v>
       </c>
-      <c r="E58" t="n">
+      <c r="F58" t="n">
         <v>1.871</v>
       </c>
-      <c r="F58" t="n">
+      <c r="G58" t="n">
         <v>0.03430051299406649</v>
       </c>
-      <c r="G58" t="n">
+      <c r="H58" t="n">
         <v>0.4866696463041895</v>
       </c>
-      <c r="H58" t="n">
+      <c r="I58" t="n">
         <v>1.871</v>
       </c>
-      <c r="I58" t="n">
+      <c r="J58" t="n">
         <v>57</v>
       </c>
-      <c r="J58" t="inlineStr">
+      <c r="K58" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K58" t="n">
+      <c r="L58" t="n">
         <v>9</v>
       </c>
     </row>
@@ -2717,33 +3007,38 @@
           <t>A10</t>
         </is>
       </c>
-      <c r="C59" t="n">
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
         <v>0.7999999999999999</v>
       </c>
-      <c r="D59" t="n">
+      <c r="E59" t="n">
         <v>0.3930000000000001</v>
       </c>
-      <c r="E59" t="n">
+      <c r="F59" t="n">
         <v>1.871</v>
       </c>
-      <c r="F59" t="n">
+      <c r="G59" t="n">
         <v>0.7593005129940665</v>
       </c>
-      <c r="G59" t="n">
+      <c r="H59" t="n">
         <v>0.3586696463041897</v>
       </c>
-      <c r="H59" t="n">
+      <c r="I59" t="n">
         <v>1.871</v>
       </c>
-      <c r="I59" t="n">
+      <c r="J59" t="n">
         <v>58</v>
       </c>
-      <c r="J59" t="inlineStr">
+      <c r="K59" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K59" t="n">
+      <c r="L59" t="n">
         <v>10</v>
       </c>
     </row>
@@ -2756,33 +3051,38 @@
           <t>A11</t>
         </is>
       </c>
-      <c r="C60" t="n">
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
         <v>0.495</v>
       </c>
-      <c r="D60" t="n">
+      <c r="E60" t="n">
         <v>0.1549999999999999</v>
       </c>
-      <c r="E60" t="n">
+      <c r="F60" t="n">
         <v>1.871</v>
       </c>
-      <c r="F60" t="n">
+      <c r="G60" t="n">
         <v>0.4543005129940665</v>
       </c>
-      <c r="G60" t="n">
+      <c r="H60" t="n">
         <v>0.1206696463041894</v>
       </c>
-      <c r="H60" t="n">
+      <c r="I60" t="n">
         <v>1.871</v>
       </c>
-      <c r="I60" t="n">
+      <c r="J60" t="n">
         <v>59</v>
       </c>
-      <c r="J60" t="inlineStr">
+      <c r="K60" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K60" t="n">
+      <c r="L60" t="n">
         <v>11</v>
       </c>
     </row>
@@ -2795,33 +3095,38 @@
           <t>A12</t>
         </is>
       </c>
-      <c r="C61" t="n">
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
         <v>1.39</v>
       </c>
-      <c r="D61" t="n">
+      <c r="E61" t="n">
         <v>0.1290000000000001</v>
       </c>
-      <c r="E61" t="n">
+      <c r="F61" t="n">
         <v>1.871</v>
       </c>
-      <c r="F61" t="n">
+      <c r="G61" t="n">
         <v>1.349300512994067</v>
       </c>
-      <c r="G61" t="n">
+      <c r="H61" t="n">
         <v>0.09466964630418964</v>
       </c>
-      <c r="H61" t="n">
+      <c r="I61" t="n">
         <v>1.871</v>
       </c>
-      <c r="I61" t="n">
+      <c r="J61" t="n">
         <v>60</v>
       </c>
-      <c r="J61" t="inlineStr">
+      <c r="K61" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K61" t="n">
+      <c r="L61" t="n">
         <v>12</v>
       </c>
     </row>
@@ -2834,33 +3139,38 @@
           <t>A13</t>
         </is>
       </c>
-      <c r="C62" t="n">
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
         <v>0.208</v>
       </c>
-      <c r="D62" t="n">
+      <c r="E62" t="n">
         <v>0.117</v>
       </c>
-      <c r="E62" t="n">
+      <c r="F62" t="n">
         <v>1.871</v>
       </c>
-      <c r="F62" t="n">
+      <c r="G62" t="n">
         <v>0.1673005129940665</v>
       </c>
-      <c r="G62" t="n">
+      <c r="H62" t="n">
         <v>0.08266964630418956</v>
       </c>
-      <c r="H62" t="n">
+      <c r="I62" t="n">
         <v>1.871</v>
       </c>
-      <c r="I62" t="n">
+      <c r="J62" t="n">
         <v>61</v>
       </c>
-      <c r="J62" t="inlineStr">
+      <c r="K62" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K62" t="n">
+      <c r="L62" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2873,33 +3183,38 @@
           <t>B17</t>
         </is>
       </c>
-      <c r="C63" t="n">
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
         <v>1.37</v>
       </c>
-      <c r="D63" t="n">
+      <c r="E63" t="n">
         <v>0.8739999999999999</v>
       </c>
-      <c r="E63" t="n">
+      <c r="F63" t="n">
         <v>1.689</v>
       </c>
-      <c r="F63" t="n">
+      <c r="G63" t="n">
         <v>1.388246290069821</v>
       </c>
-      <c r="G63" t="n">
+      <c r="H63" t="n">
         <v>0.8329727745163288</v>
       </c>
-      <c r="H63" t="n">
+      <c r="I63" t="n">
         <v>1.698580349057705</v>
       </c>
-      <c r="I63" t="n">
+      <c r="J63" t="n">
         <v>62</v>
       </c>
-      <c r="J63" t="inlineStr">
+      <c r="K63" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K63" t="n">
+      <c r="L63" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2912,33 +3227,38 @@
           <t>C17</t>
         </is>
       </c>
-      <c r="C64" t="n">
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>front</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
         <v>0.7989999999999999</v>
       </c>
-      <c r="D64" t="n">
+      <c r="E64" t="n">
         <v>0.028</v>
       </c>
-      <c r="E64" t="n">
+      <c r="F64" t="n">
         <v>1.691</v>
       </c>
-      <c r="F64" t="n">
+      <c r="G64" t="n">
         <v>0.8057845145047688</v>
       </c>
-      <c r="G64" t="n">
+      <c r="H64" t="n">
         <v>-0.04119474354982523</v>
       </c>
-      <c r="H64" t="n">
+      <c r="I64" t="n">
         <v>1.700243858954716</v>
       </c>
-      <c r="I64" t="n">
+      <c r="J64" t="n">
         <v>63</v>
       </c>
-      <c r="J64" t="inlineStr">
+      <c r="K64" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K64" t="n">
+      <c r="L64" t="n">
         <v>15</v>
       </c>
     </row>
@@ -2951,33 +3271,38 @@
           <t>D17</t>
         </is>
       </c>
-      <c r="C65" t="n">
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
         <v>0.028</v>
       </c>
-      <c r="D65" t="n">
+      <c r="E65" t="n">
         <v>0.6769999999999999</v>
       </c>
-      <c r="E65" t="n">
+      <c r="F65" t="n">
         <v>1.69</v>
       </c>
-      <c r="F65" t="n">
+      <c r="G65" t="n">
         <v>0.01239181766439332</v>
       </c>
-      <c r="G65" t="n">
+      <c r="H65" t="n">
         <v>0.6397837148545086</v>
       </c>
-      <c r="H65" t="n">
+      <c r="I65" t="n">
         <v>1.677447470343756</v>
       </c>
-      <c r="I65" t="n">
+      <c r="J65" t="n">
         <v>64</v>
       </c>
-      <c r="J65" t="inlineStr">
+      <c r="K65" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="K65" t="n">
+      <c r="L65" t="n">
         <v>16</v>
       </c>
     </row>

</xml_diff>